<commit_message>
finish and debug chemical sample Excel import
</commit_message>
<xml_diff>
--- a/rotmic/static/uploadexample_chemicalsample.xlsx
+++ b/rotmic/static/uploadexample_chemicalsample.xlsx
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="44">
   <si>
     <t>Description</t>
   </si>
@@ -140,9 +140,6 @@
     <t>Aliquotes</t>
   </si>
   <si>
-    <t>SB_D01</t>
-  </si>
-  <si>
     <t>2013-12-03</t>
   </si>
   <si>
@@ -158,9 +155,6 @@
     <t>µg</t>
   </si>
   <si>
-    <t>A11</t>
-  </si>
-  <si>
     <t>Import of Chemical (Reagent) Samples</t>
   </si>
   <si>
@@ -189,6 +183,9 @@
   </si>
   <si>
     <t>test Chemical sample</t>
+  </si>
+  <si>
+    <t>chemA_E</t>
   </si>
 </sst>
 </file>
@@ -603,7 +600,7 @@
   <dimension ref="A1:L43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -624,7 +621,7 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -634,7 +631,7 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -651,7 +648,7 @@
         <v>7</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F5" s="8" t="s">
         <v>8</v>
@@ -676,20 +673,20 @@
       </c>
     </row>
     <row r="6" spans="1:12">
-      <c r="A6" t="s">
-        <v>34</v>
+      <c r="A6">
+        <v>1</v>
       </c>
       <c r="B6" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>29</v>
-      </c>
       <c r="E6" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F6" s="7">
         <v>5</v>
@@ -704,7 +701,7 @@
         <v>26</v>
       </c>
       <c r="L6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -1219,7 +1216,7 @@
         <v>19</v>
       </c>
       <c r="E5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L5" t="s">
         <v>3</v>
@@ -1233,7 +1230,7 @@
         <v>20</v>
       </c>
       <c r="E6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="L6" t="s">
         <v>3</v>
@@ -1247,7 +1244,7 @@
         <v>21</v>
       </c>
       <c r="E7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="L7" t="s">
         <v>3</v>
@@ -1261,7 +1258,7 @@
         <v>22</v>
       </c>
       <c r="E8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="L8" t="s">
         <v>3</v>
@@ -1299,7 +1296,7 @@
     </row>
     <row r="12" spans="1:12">
       <c r="E12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="L12" t="s">
         <v>3</v>
@@ -1307,7 +1304,7 @@
     </row>
     <row r="13" spans="1:12">
       <c r="E13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L13" t="s">
         <v>3</v>
@@ -1315,7 +1312,7 @@
     </row>
     <row r="14" spans="1:12">
       <c r="E14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L14" t="s">
         <v>3</v>
@@ -1323,7 +1320,7 @@
     </row>
     <row r="15" spans="1:12">
       <c r="E15" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L15" t="s">
         <v>3</v>
@@ -1331,7 +1328,7 @@
     </row>
     <row r="16" spans="1:12">
       <c r="E16" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="L16" t="s">
         <v>3</v>

</xml_diff>